<commit_message>
Fixed 2015 Pumphouse data to add NO_FISH to fish transect with no fish
</commit_message>
<xml_diff>
--- a/raw_data/KEEN ONE/Grabowski/2015/Pumphouse Beach/Pumphouse_Fish_1_25_17.xlsx
+++ b/raw_data/KEEN ONE/Grabowski/2015/Pumphouse Beach/Pumphouse_Fish_1_25_17.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28028"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-75" yWindow="0" windowWidth="18120" windowHeight="16440"/>
+    <workbookView xWindow="2900" yWindow="0" windowWidth="25600" windowHeight="16060"/>
   </bookViews>
   <sheets>
     <sheet name="Data Entry" sheetId="1" r:id="rId1"/>
@@ -208,7 +208,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="144">
   <si>
     <t>YEAR</t>
   </si>
@@ -637,6 +637,9 @@
   </si>
   <si>
     <t>SJTMC</t>
+  </si>
+  <si>
+    <t>NO_FISH</t>
   </si>
 </sst>
 </file>
@@ -1168,29 +1171,29 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomLeft" activeCell="M3" sqref="M3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
   <cols>
-    <col min="2" max="2" width="9.140625" style="9" customWidth="1"/>
-    <col min="3" max="3" width="9.140625" style="17" customWidth="1"/>
-    <col min="4" max="4" width="9.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.7109375" customWidth="1"/>
-    <col min="6" max="6" width="12.7109375" style="9" customWidth="1"/>
+    <col min="2" max="2" width="9.1640625" style="9" customWidth="1"/>
+    <col min="3" max="3" width="9.1640625" style="17" customWidth="1"/>
+    <col min="4" max="4" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.6640625" customWidth="1"/>
+    <col min="6" max="6" width="12.6640625" style="9" customWidth="1"/>
     <col min="7" max="7" width="12" customWidth="1"/>
-    <col min="15" max="15" width="11.85546875" style="18" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="7.140625" customWidth="1"/>
-    <col min="18" max="18" width="16.85546875" style="9" customWidth="1"/>
+    <col min="15" max="15" width="11.83203125" style="18" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="7.1640625" customWidth="1"/>
+    <col min="18" max="18" width="16.83203125" style="9" customWidth="1"/>
     <col min="19" max="19" width="17" customWidth="1"/>
-    <col min="20" max="20" width="14.42578125" customWidth="1"/>
-    <col min="21" max="21" width="15.140625" customWidth="1"/>
-    <col min="22" max="22" width="11.42578125" customWidth="1"/>
+    <col min="20" max="20" width="14.5" customWidth="1"/>
+    <col min="21" max="21" width="15.1640625" customWidth="1"/>
+    <col min="22" max="22" width="11.5" customWidth="1"/>
     <col min="23" max="23" width="0" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" s="7" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:23" s="7" customFormat="1" ht="12.75" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1259,7 +1262,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:23">
       <c r="A2">
         <v>2015</v>
       </c>
@@ -1277,13 +1280,18 @@
       </c>
       <c r="F2" s="27">
         <v>1</v>
+      </c>
+      <c r="G2" t="s">
+        <v>143</v>
       </c>
       <c r="H2" s="9"/>
       <c r="I2" s="9"/>
       <c r="J2" s="9"/>
       <c r="K2" s="9"/>
       <c r="L2" s="9"/>
-      <c r="M2" s="9"/>
+      <c r="M2" s="9">
+        <v>0</v>
+      </c>
       <c r="N2" s="9"/>
       <c r="O2" s="19">
         <v>5.49</v>
@@ -1304,7 +1312,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:23">
       <c r="A3">
         <v>2015</v>
       </c>
@@ -1356,7 +1364,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:23">
       <c r="C4" s="16"/>
       <c r="D4" s="14"/>
       <c r="F4"/>
@@ -1369,7 +1377,7 @@
       <c r="N4" s="9"/>
       <c r="R4"/>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:23">
       <c r="C5" s="16"/>
       <c r="D5" s="14"/>
       <c r="F5"/>
@@ -1382,12 +1390,12 @@
       <c r="N5" s="9"/>
       <c r="R5"/>
     </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:23">
       <c r="C6" s="16"/>
       <c r="D6" s="14"/>
       <c r="M6" s="9"/>
     </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:23">
       <c r="C7" s="16"/>
       <c r="D7" s="14"/>
       <c r="H7" s="9"/>
@@ -1399,7 +1407,7 @@
       <c r="N7" s="9"/>
       <c r="T7" s="9"/>
     </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:23">
       <c r="C8" s="16"/>
       <c r="D8" s="14"/>
       <c r="H8" s="9"/>
@@ -1412,7 +1420,7 @@
       <c r="T8" s="9"/>
       <c r="V8" s="9"/>
     </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:23">
       <c r="C9" s="16"/>
       <c r="D9" s="14"/>
       <c r="H9" s="9"/>
@@ -1425,7 +1433,7 @@
       <c r="S9" s="9"/>
       <c r="T9" s="9"/>
     </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:23">
       <c r="C10" s="16"/>
       <c r="D10" s="14"/>
       <c r="H10" s="9"/>
@@ -1437,7 +1445,7 @@
       <c r="N10" s="9"/>
       <c r="T10" s="9"/>
     </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:23">
       <c r="C11" s="16"/>
       <c r="D11" s="14"/>
       <c r="H11" s="9"/>
@@ -1450,7 +1458,7 @@
       <c r="S11" s="9"/>
       <c r="T11" s="9"/>
     </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:23">
       <c r="C12" s="16"/>
       <c r="D12" s="14"/>
       <c r="H12" s="9"/>
@@ -1462,7 +1470,7 @@
       <c r="N12" s="9"/>
       <c r="T12" s="9"/>
     </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:23">
       <c r="C13" s="16"/>
       <c r="D13" s="14"/>
       <c r="H13" s="9"/>
@@ -1475,7 +1483,7 @@
       <c r="S13" s="9"/>
       <c r="T13" s="9"/>
     </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:23">
       <c r="C14" s="16"/>
       <c r="D14" s="14"/>
       <c r="H14" s="9"/>
@@ -1488,309 +1496,309 @@
       <c r="S14" s="9"/>
       <c r="T14" s="9"/>
     </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:23">
       <c r="C15" s="16"/>
       <c r="D15" s="14"/>
       <c r="T15" s="9"/>
     </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:23">
       <c r="D16" s="14"/>
       <c r="T16" s="9"/>
     </row>
-    <row r="17" spans="4:20" x14ac:dyDescent="0.2">
+    <row r="17" spans="4:20">
       <c r="D17" s="14"/>
       <c r="T17" s="9"/>
     </row>
-    <row r="18" spans="4:20" x14ac:dyDescent="0.2">
+    <row r="18" spans="4:20">
       <c r="D18" s="14"/>
       <c r="T18" s="9"/>
     </row>
-    <row r="19" spans="4:20" x14ac:dyDescent="0.2">
+    <row r="19" spans="4:20">
       <c r="D19" s="14"/>
       <c r="T19" s="9"/>
     </row>
-    <row r="20" spans="4:20" x14ac:dyDescent="0.2">
+    <row r="20" spans="4:20">
       <c r="D20" s="14"/>
       <c r="T20" s="9"/>
     </row>
-    <row r="21" spans="4:20" x14ac:dyDescent="0.2">
+    <row r="21" spans="4:20">
       <c r="D21" s="14"/>
       <c r="T21" s="9"/>
     </row>
-    <row r="22" spans="4:20" x14ac:dyDescent="0.2">
+    <row r="22" spans="4:20">
       <c r="D22" s="14"/>
       <c r="T22" s="9"/>
     </row>
-    <row r="23" spans="4:20" x14ac:dyDescent="0.2">
+    <row r="23" spans="4:20">
       <c r="D23" s="14"/>
       <c r="T23" s="9"/>
     </row>
-    <row r="7061" spans="23:23" x14ac:dyDescent="0.2">
+    <row r="7061" spans="23:23">
       <c r="W7061" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="7062" spans="23:23" x14ac:dyDescent="0.2">
+    <row r="7062" spans="23:23">
       <c r="W7062" s="11" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="7063" spans="23:23" x14ac:dyDescent="0.2">
+    <row r="7063" spans="23:23">
       <c r="W7063" s="11" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="7064" spans="23:23" x14ac:dyDescent="0.2">
+    <row r="7064" spans="23:23">
       <c r="W7064" s="11" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="7065" spans="23:23" x14ac:dyDescent="0.2">
+    <row r="7065" spans="23:23">
       <c r="W7065" s="11" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="7066" spans="23:23" x14ac:dyDescent="0.2">
+    <row r="7066" spans="23:23">
       <c r="W7066" s="11" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="7067" spans="23:23" x14ac:dyDescent="0.2">
+    <row r="7067" spans="23:23">
       <c r="W7067" s="11" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="7068" spans="23:23" x14ac:dyDescent="0.2">
+    <row r="7068" spans="23:23">
       <c r="W7068" s="12" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="7069" spans="23:23" x14ac:dyDescent="0.2">
+    <row r="7069" spans="23:23">
       <c r="W7069" s="11" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="7070" spans="23:23" x14ac:dyDescent="0.2">
+    <row r="7070" spans="23:23">
       <c r="W7070" s="11" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="7071" spans="23:23" x14ac:dyDescent="0.2">
+    <row r="7071" spans="23:23">
       <c r="W7071" s="11" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="7072" spans="23:23" x14ac:dyDescent="0.2">
+    <row r="7072" spans="23:23">
       <c r="W7072" s="11" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="7073" spans="23:23" x14ac:dyDescent="0.2">
+    <row r="7073" spans="23:23">
       <c r="W7073" s="11" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="7074" spans="23:23" x14ac:dyDescent="0.2">
+    <row r="7074" spans="23:23">
       <c r="W7074" s="11" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="7075" spans="23:23" x14ac:dyDescent="0.2">
+    <row r="7075" spans="23:23">
       <c r="W7075" s="11" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="7076" spans="23:23" x14ac:dyDescent="0.2">
+    <row r="7076" spans="23:23">
       <c r="W7076" s="11" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="7077" spans="23:23" x14ac:dyDescent="0.2">
+    <row r="7077" spans="23:23">
       <c r="W7077" s="11" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="7078" spans="23:23" x14ac:dyDescent="0.2">
+    <row r="7078" spans="23:23">
       <c r="W7078" s="11" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="7079" spans="23:23" x14ac:dyDescent="0.2">
+    <row r="7079" spans="23:23">
       <c r="W7079" s="12" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="7080" spans="23:23" x14ac:dyDescent="0.2">
+    <row r="7080" spans="23:23">
       <c r="W7080" s="11" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="7081" spans="23:23" x14ac:dyDescent="0.2">
+    <row r="7081" spans="23:23">
       <c r="W7081" s="11" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="7082" spans="23:23" x14ac:dyDescent="0.2">
+    <row r="7082" spans="23:23">
       <c r="W7082" s="11" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="7083" spans="23:23" x14ac:dyDescent="0.2">
+    <row r="7083" spans="23:23">
       <c r="W7083" s="11" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="7084" spans="23:23" x14ac:dyDescent="0.2">
+    <row r="7084" spans="23:23">
       <c r="W7084" s="11" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="7085" spans="23:23" x14ac:dyDescent="0.2">
+    <row r="7085" spans="23:23">
       <c r="W7085" s="11" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="7086" spans="23:23" x14ac:dyDescent="0.2">
+    <row r="7086" spans="23:23">
       <c r="W7086" s="11" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="7087" spans="23:23" x14ac:dyDescent="0.2">
+    <row r="7087" spans="23:23">
       <c r="W7087" s="11" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="7088" spans="23:23" x14ac:dyDescent="0.2">
+    <row r="7088" spans="23:23">
       <c r="W7088" s="11" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="7089" spans="23:23" x14ac:dyDescent="0.2">
+    <row r="7089" spans="23:23">
       <c r="W7089" s="11" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="7090" spans="23:23" x14ac:dyDescent="0.2">
+    <row r="7090" spans="23:23">
       <c r="W7090" s="11" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="7091" spans="23:23" x14ac:dyDescent="0.2">
+    <row r="7091" spans="23:23">
       <c r="W7091" s="11" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="7092" spans="23:23" x14ac:dyDescent="0.2">
+    <row r="7092" spans="23:23">
       <c r="W7092" s="12" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="7093" spans="23:23" x14ac:dyDescent="0.2">
+    <row r="7093" spans="23:23">
       <c r="W7093" s="11" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="7094" spans="23:23" x14ac:dyDescent="0.2">
+    <row r="7094" spans="23:23">
       <c r="W7094" s="11" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="7095" spans="23:23" x14ac:dyDescent="0.2">
+    <row r="7095" spans="23:23">
       <c r="W7095" s="11" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="7096" spans="23:23" x14ac:dyDescent="0.2">
+    <row r="7096" spans="23:23">
       <c r="W7096" s="11" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="7097" spans="23:23" x14ac:dyDescent="0.2">
+    <row r="7097" spans="23:23">
       <c r="W7097" s="11" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="7098" spans="23:23" x14ac:dyDescent="0.2">
+    <row r="7098" spans="23:23">
       <c r="W7098" s="11" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="7099" spans="23:23" x14ac:dyDescent="0.2">
+    <row r="7099" spans="23:23">
       <c r="W7099" s="11" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="7100" spans="23:23" x14ac:dyDescent="0.2">
+    <row r="7100" spans="23:23">
       <c r="W7100" s="11" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="7101" spans="23:23" x14ac:dyDescent="0.2">
+    <row r="7101" spans="23:23">
       <c r="W7101" s="12" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="7102" spans="23:23" x14ac:dyDescent="0.2">
+    <row r="7102" spans="23:23">
       <c r="W7102" s="11" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="7103" spans="23:23" x14ac:dyDescent="0.2">
+    <row r="7103" spans="23:23">
       <c r="W7103" s="11" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="7104" spans="23:23" x14ac:dyDescent="0.2">
+    <row r="7104" spans="23:23">
       <c r="W7104" s="11" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="7105" spans="23:23" x14ac:dyDescent="0.2">
+    <row r="7105" spans="23:23">
       <c r="W7105" s="12" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="7106" spans="23:23" x14ac:dyDescent="0.2">
+    <row r="7106" spans="23:23">
       <c r="W7106" s="11" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="7107" spans="23:23" x14ac:dyDescent="0.2">
+    <row r="7107" spans="23:23">
       <c r="W7107" s="11" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="7108" spans="23:23" x14ac:dyDescent="0.2">
+    <row r="7108" spans="23:23">
       <c r="W7108" s="11" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="7109" spans="23:23" x14ac:dyDescent="0.2">
+    <row r="7109" spans="23:23">
       <c r="W7109" s="11" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="7110" spans="23:23" x14ac:dyDescent="0.2">
+    <row r="7110" spans="23:23">
       <c r="W7110" s="13" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="7111" spans="23:23" x14ac:dyDescent="0.2">
+    <row r="7111" spans="23:23">
       <c r="W7111" s="11" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="7112" spans="23:23" x14ac:dyDescent="0.2">
+    <row r="7112" spans="23:23">
       <c r="W7112" s="11" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="7113" spans="23:23" x14ac:dyDescent="0.2">
+    <row r="7113" spans="23:23">
       <c r="W7113" s="11" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="7114" spans="23:23" x14ac:dyDescent="0.2">
+    <row r="7114" spans="23:23">
       <c r="W7114" s="11" t="s">
         <v>59</v>
       </c>
@@ -1840,19 +1848,19 @@
       <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="12" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="7.28515625" style="24" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="39.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.33203125" style="24" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="39.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4">
       <c r="B1" s="18" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="15">
       <c r="A2" s="25" t="s">
         <v>78</v>
       </c>
@@ -1864,7 +1872,7 @@
       </c>
       <c r="D2" s="20"/>
     </row>
-    <row r="3" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" ht="15">
       <c r="A3" s="25" t="s">
         <v>81</v>
       </c>
@@ -1876,7 +1884,7 @@
       </c>
       <c r="D3" s="20"/>
     </row>
-    <row r="4" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" ht="15">
       <c r="A4" s="25" t="s">
         <v>84</v>
       </c>
@@ -1888,7 +1896,7 @@
       </c>
       <c r="D4" s="20"/>
     </row>
-    <row r="5" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" ht="15">
       <c r="A5" s="25" t="s">
         <v>87</v>
       </c>
@@ -1900,7 +1908,7 @@
       </c>
       <c r="D5" s="20"/>
     </row>
-    <row r="6" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" ht="15">
       <c r="A6" s="25" t="s">
         <v>90</v>
       </c>
@@ -1912,7 +1920,7 @@
       </c>
       <c r="D6" s="20"/>
     </row>
-    <row r="7" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" ht="15">
       <c r="A7" s="25" t="s">
         <v>93</v>
       </c>
@@ -1924,7 +1932,7 @@
       </c>
       <c r="D7" s="20"/>
     </row>
-    <row r="8" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" ht="15">
       <c r="A8" s="25" t="s">
         <v>95</v>
       </c>
@@ -1936,7 +1944,7 @@
       </c>
       <c r="D8" s="20"/>
     </row>
-    <row r="9" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" ht="15">
       <c r="A9" s="25" t="s">
         <v>98</v>
       </c>
@@ -1948,7 +1956,7 @@
       </c>
       <c r="D9" s="20"/>
     </row>
-    <row r="10" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" ht="15">
       <c r="A10" s="25" t="s">
         <v>101</v>
       </c>
@@ -1960,7 +1968,7 @@
       </c>
       <c r="D10" s="20"/>
     </row>
-    <row r="11" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" ht="15">
       <c r="A11" s="25" t="s">
         <v>104</v>
       </c>
@@ -1972,7 +1980,7 @@
       </c>
       <c r="D11" s="20"/>
     </row>
-    <row r="12" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" ht="15">
       <c r="A12" s="25" t="s">
         <v>105</v>
       </c>
@@ -1982,7 +1990,7 @@
       <c r="C12" s="20"/>
       <c r="D12" s="20"/>
     </row>
-    <row r="13" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" ht="15">
       <c r="A13" s="25" t="s">
         <v>107</v>
       </c>
@@ -1992,7 +2000,7 @@
       <c r="C13" s="20"/>
       <c r="D13" s="20"/>
     </row>
-    <row r="14" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" ht="15">
       <c r="A14" s="25" t="s">
         <v>109</v>
       </c>
@@ -2002,7 +2010,7 @@
       <c r="C14" s="20"/>
       <c r="D14" s="20"/>
     </row>
-    <row r="15" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" ht="15">
       <c r="A15" s="25" t="s">
         <v>111</v>
       </c>
@@ -2012,7 +2020,7 @@
       <c r="C15" s="20"/>
       <c r="D15" s="20"/>
     </row>
-    <row r="16" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" ht="15">
       <c r="A16" s="25" t="s">
         <v>113</v>
       </c>
@@ -2022,7 +2030,7 @@
       <c r="C16" s="20"/>
       <c r="D16" s="20"/>
     </row>
-    <row r="17" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" ht="15">
       <c r="A17" s="25" t="s">
         <v>115</v>
       </c>
@@ -2032,7 +2040,7 @@
       <c r="C17" s="20"/>
       <c r="D17" s="20"/>
     </row>
-    <row r="18" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" ht="15">
       <c r="A18" s="25" t="s">
         <v>117</v>
       </c>
@@ -2042,7 +2050,7 @@
       <c r="C18" s="22"/>
       <c r="D18" s="20"/>
     </row>
-    <row r="19" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" ht="15">
       <c r="A19" s="25" t="s">
         <v>119</v>
       </c>
@@ -2052,7 +2060,7 @@
       <c r="C19" s="22"/>
       <c r="D19" s="20"/>
     </row>
-    <row r="20" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" ht="15">
       <c r="A20" s="25" t="s">
         <v>93</v>
       </c>
@@ -2062,7 +2070,7 @@
       <c r="C20" s="22"/>
       <c r="D20" s="20"/>
     </row>
-    <row r="21" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" ht="15">
       <c r="A21" s="26" t="s">
         <v>121</v>
       </c>
@@ -2072,7 +2080,7 @@
       <c r="C21" s="20"/>
       <c r="D21" s="20"/>
     </row>
-    <row r="22" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" ht="15">
       <c r="A22" s="26" t="s">
         <v>123</v>
       </c>
@@ -2082,7 +2090,7 @@
       <c r="C22" s="20"/>
       <c r="D22" s="20"/>
     </row>
-    <row r="23" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" ht="15">
       <c r="A23" s="26" t="s">
         <v>125</v>
       </c>
@@ -2092,7 +2100,7 @@
       <c r="C23" s="20"/>
       <c r="D23" s="20"/>
     </row>
-    <row r="24" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" ht="15">
       <c r="A24" s="26" t="s">
         <v>127</v>
       </c>
@@ -2102,7 +2110,7 @@
       <c r="C24" s="20"/>
       <c r="D24" s="20"/>
     </row>
-    <row r="25" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" ht="15">
       <c r="A25" s="26" t="s">
         <v>129</v>
       </c>
@@ -2112,7 +2120,7 @@
       <c r="C25" s="20"/>
       <c r="D25" s="20"/>
     </row>
-    <row r="26" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" ht="15">
       <c r="A26" s="26" t="s">
         <v>131</v>
       </c>
@@ -2122,7 +2130,7 @@
       <c r="C26" s="20"/>
       <c r="D26" s="20"/>
     </row>
-    <row r="27" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" ht="15">
       <c r="A27" s="26" t="s">
         <v>133</v>
       </c>
@@ -2132,7 +2140,7 @@
       <c r="C27" s="20"/>
       <c r="D27" s="20"/>
     </row>
-    <row r="28" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" ht="15">
       <c r="A28" s="26" t="s">
         <v>135</v>
       </c>

</xml_diff>